<commit_message>
Updated readmes, incldued eBOMs, included images
</commit_message>
<xml_diff>
--- a/Production Design Projects/DAPLink/DIPDAP/v1.0.0/DIPDAP-BOM.xlsx
+++ b/Production Design Projects/DAPLink/DIPDAP/v1.0.0/DIPDAP-BOM.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstyles\Documents\mbed\Projects\AppsEng\OpenHDK\DAPlink\DIPDAP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="7356"/>
+    <workbookView xWindow="-38400" yWindow="-2740" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="DIPDAP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="100">
   <si>
     <t>Assembly</t>
   </si>
@@ -291,12 +291,6 @@
     <t>THROUGH-HOLE</t>
   </si>
   <si>
-    <t>TSW-107-02-S-S</t>
-  </si>
-  <si>
-    <t>TSW-107-02-S-S-RA</t>
-  </si>
-  <si>
     <t>Alps</t>
   </si>
   <si>
@@ -319,6 +313,12 @@
   </si>
   <si>
     <t>MCMR04X152-JTL</t>
+  </si>
+  <si>
+    <t>Samtech</t>
+  </si>
+  <si>
+    <t>TSW-107-08-G-S-RA</t>
   </si>
 </sst>
 </file>
@@ -922,7 +922,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -957,7 +957,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1134,7 +1134,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1144,24 +1144,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="22.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="22.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>1759380</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>1758947</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>1758947</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>1759380</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>1758947</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>1758947</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>1759393</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>1759381</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>2115658</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>1331502</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>1645325</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>2290329</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>2290329</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>2290329</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>1842056</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
@@ -1629,13 +1629,13 @@
         <v>402</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>17</v>
@@ -1644,7 +1644,7 @@
         <v>2072528</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1658,13 +1658,13 @@
         <v>402</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>17</v>
@@ -1673,7 +1673,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -1687,13 +1687,13 @@
         <v>402</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>17</v>
@@ -1702,7 +1702,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
@@ -1716,13 +1716,13 @@
         <v>402</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
@@ -1731,7 +1731,7 @@
         <v>2072926</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -1745,13 +1745,13 @@
         <v>402</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>17</v>
@@ -1760,7 +1760,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -1774,13 +1774,13 @@
         <v>402</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>17</v>
@@ -1789,7 +1789,7 @@
         <v>2072926</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -1803,13 +1803,13 @@
         <v>402</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>17</v>
@@ -1818,7 +1818,7 @@
         <v>2072650</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>73</v>
       </c>
@@ -1832,13 +1832,13 @@
         <v>402</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
@@ -1847,7 +1847,7 @@
         <v>2072528</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>74</v>
       </c>
@@ -1861,13 +1861,13 @@
         <v>402</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>17</v>
@@ -1876,7 +1876,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
@@ -1890,13 +1890,13 @@
         <v>402</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>17</v>
@@ -1905,7 +1905,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
@@ -1919,13 +1919,13 @@
         <v>402</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>17</v>
@@ -1934,7 +1934,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
@@ -1948,13 +1948,13 @@
         <v>402</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>17</v>
@@ -1963,7 +1963,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>78</v>
       </c>
@@ -1977,13 +1977,13 @@
         <v>402</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>17</v>
@@ -1992,7 +1992,7 @@
         <v>2073068</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>79</v>
       </c>
@@ -2006,22 +2006,22 @@
         <v>81</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -2050,24 +2050,41 @@
         <v>1056526</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="F34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="3">
+        <v>2041451</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>